<commit_message>
pokus o předělání grid na pack, release verze 3.7.4
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Sharepoint_databaze.xlsx
+++ b/TRIMAZKON/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\TRIMAZKON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBCCFAF-E71F-4896-B0B6-6242B652AFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
   <bookViews>
-    <workbookView xWindow="12435" yWindow="3795" windowWidth="28800" windowHeight="15285" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -19,17 +19,28 @@
     <sheet name="Kabely" sheetId="7" r:id="rId4"/>
     <sheet name="Přislušenství" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -1392,16 +1403,13 @@
   </si>
   <si>
     <t>EtherNet/IP module</t>
-  </si>
-  <si>
-    <t>gfsh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1517,14 +1525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1534,6 +1540,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1820,7 +1828,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -1828,18 +1836,18 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1854,7 +1862,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1869,7 +1877,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1884,7 +1892,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1899,7 +1907,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1914,7 +1922,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1929,7 +1937,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1944,7 +1952,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1959,7 +1967,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1974,7 +1982,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1984,7 +1992,7 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1994,7 +2002,7 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
@@ -2004,7 +2012,7 @@
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -2014,7 +2022,7 @@
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2024,7 +2032,7 @@
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -2034,7 +2042,7 @@
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -2044,7 +2052,7 @@
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -2054,7 +2062,7 @@
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -2064,7 +2072,7 @@
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -2074,7 +2082,7 @@
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -2084,7 +2092,7 @@
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -2094,7 +2102,7 @@
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>55</v>
       </c>
@@ -2115,34 +2123,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -2153,7 +2161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>61</v>
       </c>
@@ -2164,7 +2172,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
@@ -2175,7 +2183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2186,7 +2194,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>70</v>
       </c>
@@ -2197,7 +2205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>73</v>
       </c>
@@ -2208,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -2219,7 +2227,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>79</v>
       </c>
@@ -2230,7 +2238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>82</v>
       </c>
@@ -2239,7 +2247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>84</v>
       </c>
@@ -2250,7 +2258,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>87</v>
       </c>
@@ -2261,7 +2269,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>90</v>
       </c>
@@ -2272,7 +2280,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>93</v>
       </c>
@@ -2283,7 +2291,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>96</v>
       </c>
@@ -2294,7 +2302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
@@ -2305,7 +2313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
         <v>102</v>
       </c>
@@ -2316,7 +2324,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="8" t="s">
         <v>82</v>
       </c>
@@ -2325,7 +2333,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
         <v>106</v>
       </c>
@@ -2336,7 +2344,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
         <v>109</v>
       </c>
@@ -2347,7 +2355,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
         <v>112</v>
       </c>
@@ -2358,7 +2366,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="8" t="s">
         <v>115</v>
       </c>
@@ -2369,7 +2377,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="8" t="s">
         <v>118</v>
       </c>
@@ -2380,7 +2388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="8" t="s">
         <v>121</v>
       </c>
@@ -2391,7 +2399,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="8" t="s">
         <v>124</v>
       </c>
@@ -2402,7 +2410,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="8" t="s">
         <v>127</v>
       </c>
@@ -2413,7 +2421,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="8" t="s">
         <v>130</v>
       </c>
@@ -2424,7 +2432,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
         <v>133</v>
       </c>
@@ -2435,7 +2443,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="8" t="s">
         <v>136</v>
       </c>
@@ -2446,7 +2454,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="8" t="s">
         <v>139</v>
       </c>
@@ -2457,7 +2465,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
         <v>82</v>
       </c>
@@ -2466,7 +2474,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
         <v>143</v>
       </c>
@@ -2477,7 +2485,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
         <v>146</v>
       </c>
@@ -2488,7 +2496,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="8" t="s">
         <v>149</v>
       </c>
@@ -2499,7 +2507,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="8" t="s">
         <v>152</v>
       </c>
@@ -2510,7 +2518,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="8" t="s">
         <v>155</v>
       </c>
@@ -2521,7 +2529,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="8" t="s">
         <v>158</v>
       </c>
@@ -2532,7 +2540,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="8" t="s">
         <v>161</v>
       </c>
@@ -2543,7 +2551,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="8" t="s">
         <v>164</v>
       </c>
@@ -2554,7 +2562,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="8" t="s">
         <v>167</v>
       </c>
@@ -2565,7 +2573,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="8" t="s">
         <v>170</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="8" t="s">
         <v>173</v>
       </c>
@@ -2587,7 +2595,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="8" t="s">
         <v>176</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
         <v>179</v>
       </c>
@@ -2609,7 +2617,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="8" t="s">
         <v>182</v>
       </c>
@@ -2620,7 +2628,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
         <v>185</v>
       </c>
@@ -2631,7 +2639,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="8" t="s">
         <v>188</v>
       </c>
@@ -2642,7 +2650,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="8" t="s">
         <v>191</v>
       </c>
@@ -2653,7 +2661,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="8" t="s">
         <v>194</v>
       </c>
@@ -2664,7 +2672,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="8" t="s">
         <v>197</v>
       </c>
@@ -2675,7 +2683,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="8" t="s">
         <v>200</v>
       </c>
@@ -2686,7 +2694,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="8" t="s">
         <v>203</v>
       </c>
@@ -2697,7 +2705,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
         <v>206</v>
       </c>
@@ -2708,7 +2716,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="8" t="s">
         <v>209</v>
       </c>
@@ -2719,7 +2727,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="8" t="s">
         <v>212</v>
       </c>
@@ -2730,7 +2738,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="8" t="s">
         <v>215</v>
       </c>
@@ -2741,7 +2749,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
         <v>218</v>
       </c>
@@ -2752,7 +2760,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="8" t="s">
         <v>221</v>
       </c>
@@ -2763,7 +2771,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="8" t="s">
         <v>224</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="8" t="s">
         <v>227</v>
       </c>
@@ -2785,7 +2793,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="8" t="s">
         <v>230</v>
       </c>
@@ -2796,7 +2804,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="8" t="s">
         <v>233</v>
       </c>
@@ -2807,7 +2815,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="8" t="s">
         <v>236</v>
       </c>
@@ -2818,7 +2826,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="8" t="s">
         <v>239</v>
       </c>
@@ -2829,7 +2837,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="8" t="s">
         <v>242</v>
       </c>
@@ -2840,7 +2848,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="8" t="s">
         <v>245</v>
       </c>
@@ -2851,7 +2859,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="8" t="s">
         <v>248</v>
       </c>
@@ -2862,7 +2870,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="8" t="s">
         <v>251</v>
       </c>
@@ -2873,7 +2881,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="8" t="s">
         <v>254</v>
       </c>
@@ -2884,7 +2892,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="8" t="s">
         <v>257</v>
       </c>
@@ -2895,7 +2903,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="8" t="s">
         <v>260</v>
       </c>
@@ -2906,7 +2914,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="8" t="s">
         <v>263</v>
       </c>
@@ -2917,7 +2925,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="8" t="s">
         <v>266</v>
       </c>
@@ -2928,7 +2936,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="8" t="s">
         <v>269</v>
       </c>
@@ -2939,7 +2947,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="8" t="s">
         <v>272</v>
       </c>
@@ -2950,7 +2958,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="8" t="s">
         <v>275</v>
       </c>
@@ -2961,7 +2969,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="8" t="s">
         <v>278</v>
       </c>
@@ -2972,7 +2980,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="8" t="s">
         <v>281</v>
       </c>
@@ -2983,7 +2991,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="8" t="s">
         <v>284</v>
       </c>
@@ -2994,7 +3002,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="8" t="s">
         <v>287</v>
       </c>
@@ -3005,7 +3013,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="8" t="s">
         <v>290</v>
       </c>
@@ -3016,7 +3024,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="8" t="s">
         <v>293</v>
       </c>
@@ -3027,7 +3035,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="8" t="s">
         <v>296</v>
       </c>
@@ -3038,7 +3046,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="8" t="s">
         <v>299</v>
       </c>
@@ -3049,7 +3057,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="8" t="s">
         <v>302</v>
       </c>
@@ -3060,7 +3068,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="8" t="s">
         <v>305</v>
       </c>
@@ -3071,7 +3079,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="8" t="s">
         <v>308</v>
       </c>
@@ -3082,7 +3090,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="8" t="s">
         <v>311</v>
       </c>
@@ -3107,11 +3115,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="150.5703125" customWidth="1"/>
@@ -3119,17 +3127,17 @@
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>315</v>
       </c>
@@ -3144,7 +3152,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>318</v>
       </c>
@@ -3159,7 +3167,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>321</v>
       </c>
@@ -3174,7 +3182,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>324</v>
       </c>
@@ -3189,7 +3197,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -3204,7 +3212,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -3219,7 +3227,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>333</v>
       </c>
@@ -3234,7 +3242,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -3249,7 +3257,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>339</v>
       </c>
@@ -3264,7 +3272,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>342</v>
       </c>
@@ -3272,7 +3280,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>344</v>
       </c>
@@ -3280,7 +3288,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>346</v>
       </c>
@@ -3289,12 +3297,12 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>348</v>
       </c>
@@ -3302,7 +3310,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>350</v>
       </c>
@@ -3311,7 +3319,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>352</v>
       </c>
@@ -3319,7 +3327,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>354</v>
       </c>
@@ -3327,7 +3335,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>356</v>
       </c>
@@ -3335,7 +3343,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>358</v>
       </c>
@@ -3343,7 +3351,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>360</v>
       </c>
@@ -3351,7 +3359,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>362</v>
       </c>
@@ -3359,7 +3367,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>364</v>
       </c>
@@ -3367,7 +3375,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>366</v>
       </c>
@@ -3375,7 +3383,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -3383,7 +3391,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>370</v>
       </c>
@@ -3391,7 +3399,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>372</v>
       </c>
@@ -3399,7 +3407,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>372</v>
       </c>
@@ -3407,12 +3415,9 @@
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>375</v>
-      </c>
-      <c r="B29" t="s">
-        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3432,23 +3437,23 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="134.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>376</v>
       </c>
@@ -3456,7 +3461,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>378</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>380</v>
       </c>
@@ -3472,7 +3477,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>382</v>
       </c>
@@ -3480,7 +3485,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>384</v>
       </c>
@@ -3488,7 +3493,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>386</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>388</v>
       </c>
@@ -3504,7 +3509,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>390</v>
       </c>
@@ -3512,7 +3517,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>392</v>
       </c>
@@ -3520,7 +3525,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>394</v>
       </c>
@@ -3528,7 +3533,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>396</v>
       </c>
@@ -3536,7 +3541,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>398</v>
       </c>
@@ -3544,7 +3549,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>400</v>
       </c>
@@ -3552,7 +3557,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>402</v>
       </c>
@@ -3560,7 +3565,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>404</v>
       </c>
@@ -3568,7 +3573,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
         <v>406</v>
       </c>
@@ -3576,7 +3581,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
         <v>408</v>
       </c>
@@ -3584,7 +3589,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
         <v>410</v>
       </c>
@@ -3606,10 +3611,10 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -3617,17 +3622,17 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
         <v>412</v>
       </c>
@@ -3638,7 +3643,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -3649,7 +3654,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>414</v>
       </c>
@@ -3659,7 +3664,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>415</v>
       </c>
@@ -3669,7 +3674,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>416</v>
       </c>
@@ -3679,7 +3684,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>417</v>
       </c>
@@ -3689,7 +3694,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>418</v>
       </c>
@@ -3699,7 +3704,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>419</v>
       </c>
@@ -3709,7 +3714,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>420</v>
       </c>
@@ -3723,7 +3728,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -3737,7 +3742,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="C12" s="6" t="s">
         <v>428</v>
       </c>
@@ -3745,7 +3750,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="6" t="s">
         <v>430</v>
       </c>
@@ -3753,7 +3758,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
         <v>432</v>
       </c>
@@ -3761,7 +3766,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="C15" s="6" t="s">
         <v>434</v>
       </c>
@@ -3769,7 +3774,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="C16" s="6" t="s">
         <v>436</v>
       </c>
@@ -3777,7 +3782,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="C17" s="6" t="s">
         <v>438</v>
       </c>
@@ -3785,7 +3790,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="C18" s="6" t="s">
         <v>440</v>
       </c>
@@ -3793,7 +3798,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="C19" s="1" t="s">
         <v>442</v>
       </c>
@@ -3801,7 +3806,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4">
       <c r="C20" s="1" t="s">
         <v>444</v>
       </c>
@@ -3809,7 +3814,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4">
       <c r="C21" s="1" t="s">
         <v>446</v>
       </c>
@@ -3817,7 +3822,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4">
       <c r="C22" s="1" t="s">
         <v>448</v>
       </c>
@@ -3825,22 +3830,22 @@
         <v>449</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -4102,39 +4107,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
 </file>
</xml_diff>

<commit_message>
práce na zobrazení podrobných dat v katalog makeru
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Sharepoint_databaze.xlsx
+++ b/TRIMAZKON/Sharepoint_databaze.xlsx
@@ -1,46 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\TRIMAZKON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E5D8A-1851-489A-A445-7DE1A96A1FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
     <sheet name="Optika" sheetId="6" r:id="rId2"/>
-    <sheet name="Kamery" sheetId="3" r:id="rId3"/>
-    <sheet name="Kabely" sheetId="7" r:id="rId4"/>
-    <sheet name="Přislušenství" sheetId="4" r:id="rId5"/>
+    <sheet name="Světla" sheetId="8" r:id="rId3"/>
+    <sheet name="Kamery" sheetId="3" r:id="rId4"/>
+    <sheet name="Kabely" sheetId="7" r:id="rId5"/>
+    <sheet name="Přislušenství" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="461">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -1403,13 +1393,46 @@
   </si>
   <si>
     <t>EtherNet/IP module</t>
+  </si>
+  <si>
+    <t>všichni výrobci</t>
+  </si>
+  <si>
+    <t>LL-130W</t>
+  </si>
+  <si>
+    <t>LA-120W</t>
+  </si>
+  <si>
+    <t>DLU-140W-HI</t>
+  </si>
+  <si>
+    <t>CL-50</t>
+  </si>
+  <si>
+    <t>LA-70W</t>
+  </si>
+  <si>
+    <t>BL-50W-4S</t>
+  </si>
+  <si>
+    <t>SP-27IR-850</t>
+  </si>
+  <si>
+    <t>LA-70B</t>
+  </si>
+  <si>
+    <t>DL-120W-HI</t>
+  </si>
+  <si>
+    <t>FL-MD90MC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1525,12 +1548,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1540,8 +1565,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1828,7 +1851,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -1836,18 +1859,18 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1862,7 +1885,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1877,7 +1900,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1892,7 +1915,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +1930,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +1945,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1937,7 +1960,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1952,7 +1975,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1967,7 +1990,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -1982,7 +2005,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1992,7 +2015,7 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -2002,7 +2025,7 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
@@ -2012,7 +2035,7 @@
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -2022,7 +2045,7 @@
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2032,7 +2055,7 @@
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -2042,7 +2065,7 @@
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -2052,7 +2075,7 @@
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -2062,7 +2085,7 @@
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -2072,7 +2095,7 @@
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -2082,7 +2105,7 @@
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -2092,7 +2115,7 @@
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -2102,7 +2125,7 @@
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>55</v>
       </c>
@@ -2123,34 +2146,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -2161,7 +2184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>61</v>
       </c>
@@ -2172,7 +2195,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
@@ -2183,7 +2206,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2194,7 +2217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>70</v>
       </c>
@@ -2205,7 +2228,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>73</v>
       </c>
@@ -2216,7 +2239,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -2227,7 +2250,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>79</v>
       </c>
@@ -2238,7 +2261,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>82</v>
       </c>
@@ -2247,7 +2270,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>84</v>
       </c>
@@ -2258,7 +2281,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>87</v>
       </c>
@@ -2269,7 +2292,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>90</v>
       </c>
@@ -2280,7 +2303,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>93</v>
       </c>
@@ -2291,7 +2314,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>96</v>
       </c>
@@ -2302,7 +2325,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
@@ -2313,7 +2336,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>102</v>
       </c>
@@ -2324,7 +2347,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>82</v>
       </c>
@@ -2333,7 +2356,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>106</v>
       </c>
@@ -2344,7 +2367,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>109</v>
       </c>
@@ -2355,7 +2378,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>112</v>
       </c>
@@ -2366,7 +2389,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>115</v>
       </c>
@@ -2377,7 +2400,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>118</v>
       </c>
@@ -2388,7 +2411,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>121</v>
       </c>
@@ -2399,7 +2422,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>124</v>
       </c>
@@ -2410,7 +2433,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>127</v>
       </c>
@@ -2421,7 +2444,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>130</v>
       </c>
@@ -2432,7 +2455,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>133</v>
       </c>
@@ -2443,7 +2466,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>136</v>
       </c>
@@ -2454,7 +2477,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>139</v>
       </c>
@@ -2465,7 +2488,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>82</v>
       </c>
@@ -2474,7 +2497,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>143</v>
       </c>
@@ -2485,7 +2508,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>146</v>
       </c>
@@ -2496,7 +2519,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>149</v>
       </c>
@@ -2507,7 +2530,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>152</v>
       </c>
@@ -2518,7 +2541,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>155</v>
       </c>
@@ -2529,7 +2552,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>158</v>
       </c>
@@ -2540,7 +2563,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>161</v>
       </c>
@@ -2551,7 +2574,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>164</v>
       </c>
@@ -2562,7 +2585,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>167</v>
       </c>
@@ -2573,7 +2596,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>170</v>
       </c>
@@ -2584,7 +2607,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>173</v>
       </c>
@@ -2595,7 +2618,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>176</v>
       </c>
@@ -2606,7 +2629,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>179</v>
       </c>
@@ -2617,7 +2640,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>182</v>
       </c>
@@ -2628,7 +2651,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>185</v>
       </c>
@@ -2639,7 +2662,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>188</v>
       </c>
@@ -2650,7 +2673,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>191</v>
       </c>
@@ -2661,7 +2684,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>194</v>
       </c>
@@ -2672,7 +2695,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>197</v>
       </c>
@@ -2683,7 +2706,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>200</v>
       </c>
@@ -2694,7 +2717,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>203</v>
       </c>
@@ -2705,7 +2728,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>206</v>
       </c>
@@ -2716,7 +2739,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>209</v>
       </c>
@@ -2727,7 +2750,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>212</v>
       </c>
@@ -2738,7 +2761,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>215</v>
       </c>
@@ -2749,7 +2772,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>218</v>
       </c>
@@ -2760,7 +2783,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>221</v>
       </c>
@@ -2771,7 +2794,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>224</v>
       </c>
@@ -2782,7 +2805,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>227</v>
       </c>
@@ -2793,7 +2816,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>230</v>
       </c>
@@ -2804,7 +2827,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>233</v>
       </c>
@@ -2815,7 +2838,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>236</v>
       </c>
@@ -2826,7 +2849,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>239</v>
       </c>
@@ -2837,7 +2860,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>242</v>
       </c>
@@ -2848,7 +2871,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>245</v>
       </c>
@@ -2859,7 +2882,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>248</v>
       </c>
@@ -2870,7 +2893,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>251</v>
       </c>
@@ -2881,7 +2904,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>254</v>
       </c>
@@ -2892,7 +2915,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>257</v>
       </c>
@@ -2903,7 +2926,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>260</v>
       </c>
@@ -2914,7 +2937,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>263</v>
       </c>
@@ -2925,7 +2948,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>266</v>
       </c>
@@ -2936,7 +2959,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>269</v>
       </c>
@@ -2947,7 +2970,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>272</v>
       </c>
@@ -2958,7 +2981,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>275</v>
       </c>
@@ -2969,7 +2992,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>278</v>
       </c>
@@ -2980,7 +3003,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>281</v>
       </c>
@@ -2991,7 +3014,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>284</v>
       </c>
@@ -3002,7 +3025,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>287</v>
       </c>
@@ -3013,7 +3036,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>290</v>
       </c>
@@ -3024,7 +3047,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>293</v>
       </c>
@@ -3035,7 +3058,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>296</v>
       </c>
@@ -3046,7 +3069,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>299</v>
       </c>
@@ -3057,7 +3080,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>302</v>
       </c>
@@ -3068,7 +3091,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>305</v>
       </c>
@@ -3079,7 +3102,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>308</v>
       </c>
@@ -3090,7 +3113,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>311</v>
       </c>
@@ -3112,6 +3135,86 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEEB26D-9786-4470-A8AD-43264E85ECB9}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -3119,7 +3222,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="150.5703125" customWidth="1"/>
@@ -3127,17 +3230,17 @@
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>315</v>
       </c>
@@ -3152,7 +3255,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>318</v>
       </c>
@@ -3167,7 +3270,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>321</v>
       </c>
@@ -3182,7 +3285,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>324</v>
       </c>
@@ -3197,7 +3300,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -3212,7 +3315,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>330</v>
       </c>
@@ -3227,7 +3330,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>333</v>
       </c>
@@ -3242,7 +3345,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>336</v>
       </c>
@@ -3257,7 +3360,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>339</v>
       </c>
@@ -3272,7 +3375,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>342</v>
       </c>
@@ -3280,7 +3383,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>344</v>
       </c>
@@ -3288,7 +3391,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>346</v>
       </c>
@@ -3297,12 +3400,12 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>348</v>
       </c>
@@ -3310,7 +3413,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>350</v>
       </c>
@@ -3319,7 +3422,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>352</v>
       </c>
@@ -3327,7 +3430,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>354</v>
       </c>
@@ -3335,7 +3438,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>356</v>
       </c>
@@ -3343,7 +3446,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>358</v>
       </c>
@@ -3351,7 +3454,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>360</v>
       </c>
@@ -3359,7 +3462,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>362</v>
       </c>
@@ -3367,7 +3470,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>364</v>
       </c>
@@ -3375,7 +3478,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>366</v>
       </c>
@@ -3383,7 +3486,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -3391,7 +3494,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>370</v>
       </c>
@@ -3399,7 +3502,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>372</v>
       </c>
@@ -3407,7 +3510,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>372</v>
       </c>
@@ -3415,7 +3518,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>375</v>
       </c>
@@ -3429,7 +3532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F3B6E1-C926-490E-B179-CA4119029E15}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -3437,23 +3540,23 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="134.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>376</v>
       </c>
@@ -3461,7 +3564,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>378</v>
       </c>
@@ -3469,7 +3572,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>380</v>
       </c>
@@ -3477,7 +3580,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>382</v>
       </c>
@@ -3485,7 +3588,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>384</v>
       </c>
@@ -3493,7 +3596,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>386</v>
       </c>
@@ -3501,7 +3604,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>388</v>
       </c>
@@ -3509,7 +3612,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>390</v>
       </c>
@@ -3517,7 +3620,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>392</v>
       </c>
@@ -3525,7 +3628,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>394</v>
       </c>
@@ -3533,7 +3636,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>396</v>
       </c>
@@ -3541,7 +3644,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>398</v>
       </c>
@@ -3549,7 +3652,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>400</v>
       </c>
@@ -3557,7 +3660,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>402</v>
       </c>
@@ -3565,7 +3668,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>404</v>
       </c>
@@ -3573,7 +3676,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>406</v>
       </c>
@@ -3581,7 +3684,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>408</v>
       </c>
@@ -3589,7 +3692,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>410</v>
       </c>
@@ -3606,15 +3709,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -3622,17 +3725,17 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>412</v>
       </c>
@@ -3643,7 +3746,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -3654,7 +3757,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>414</v>
       </c>
@@ -3664,7 +3767,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>415</v>
       </c>
@@ -3674,7 +3777,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>416</v>
       </c>
@@ -3684,7 +3787,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>417</v>
       </c>
@@ -3694,7 +3797,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>418</v>
       </c>
@@ -3704,7 +3807,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>419</v>
       </c>
@@ -3714,7 +3817,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>420</v>
       </c>
@@ -3728,7 +3831,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -3742,7 +3845,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>428</v>
       </c>
@@ -3750,7 +3853,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>430</v>
       </c>
@@ -3758,7 +3861,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>432</v>
       </c>
@@ -3766,7 +3869,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
         <v>434</v>
       </c>
@@ -3774,7 +3877,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>436</v>
       </c>
@@ -3782,7 +3885,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
         <v>438</v>
       </c>
@@ -3790,7 +3893,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
         <v>440</v>
       </c>
@@ -3798,7 +3901,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>442</v>
       </c>
@@ -3806,7 +3909,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>444</v>
       </c>
@@ -3814,7 +3917,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>446</v>
       </c>
@@ -3822,7 +3925,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>448</v>
       </c>
@@ -3830,22 +3933,22 @@
         <v>449</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -3858,26 +3961,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
     <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
@@ -4106,14 +4189,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
+    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
+    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
release verze 4.0.0, oprava dopadů zoomu na ip setting
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Sharepoint_databaze.xlsx
+++ b/TRIMAZKON/Sharepoint_databaze.xlsx
@@ -1,36 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\TRIMAZKON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E5D8A-1851-489A-A445-7DE1A96A1FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
     <sheet name="Optika" sheetId="6" r:id="rId2"/>
-    <sheet name="Světla" sheetId="8" r:id="rId3"/>
-    <sheet name="Kamery" sheetId="3" r:id="rId4"/>
-    <sheet name="Kabely" sheetId="7" r:id="rId5"/>
-    <sheet name="Přislušenství" sheetId="4" r:id="rId6"/>
+    <sheet name="Kamery" sheetId="3" r:id="rId3"/>
+    <sheet name="Kabely" sheetId="7" r:id="rId4"/>
+    <sheet name="Přislušenství" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -1393,46 +1403,13 @@
   </si>
   <si>
     <t>EtherNet/IP module</t>
-  </si>
-  <si>
-    <t>všichni výrobci</t>
-  </si>
-  <si>
-    <t>LL-130W</t>
-  </si>
-  <si>
-    <t>LA-120W</t>
-  </si>
-  <si>
-    <t>DLU-140W-HI</t>
-  </si>
-  <si>
-    <t>CL-50</t>
-  </si>
-  <si>
-    <t>LA-70W</t>
-  </si>
-  <si>
-    <t>BL-50W-4S</t>
-  </si>
-  <si>
-    <t>SP-27IR-850</t>
-  </si>
-  <si>
-    <t>LA-70B</t>
-  </si>
-  <si>
-    <t>DL-120W-HI</t>
-  </si>
-  <si>
-    <t>FL-MD90MC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1548,14 +1525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1565,6 +1540,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1851,7 +1828,7 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" customWidth="1"/>
@@ -1859,18 +1836,18 @@
     <col min="4" max="4" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1885,7 +1862,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1900,7 +1877,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1915,7 +1892,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1930,7 +1907,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1945,7 +1922,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -1960,7 +1937,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1975,7 +1952,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1990,7 +1967,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -2005,7 +1982,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -2015,7 +1992,7 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -2025,7 +2002,7 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>37</v>
       </c>
@@ -2035,7 +2012,7 @@
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
@@ -2045,7 +2022,7 @@
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2055,7 +2032,7 @@
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
@@ -2065,7 +2042,7 @@
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -2075,7 +2052,7 @@
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -2085,7 +2062,7 @@
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -2095,7 +2072,7 @@
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -2105,7 +2082,7 @@
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -2115,7 +2092,7 @@
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -2125,7 +2102,7 @@
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
         <v>55</v>
       </c>
@@ -2146,34 +2123,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6243DA3-0875-4C03-8E69-F223C9363894}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="17"/>
       <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>58</v>
       </c>
@@ -2184,7 +2161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>61</v>
       </c>
@@ -2195,7 +2172,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
@@ -2206,7 +2183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2217,7 +2194,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>70</v>
       </c>
@@ -2228,7 +2205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>73</v>
       </c>
@@ -2239,7 +2216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>76</v>
       </c>
@@ -2250,7 +2227,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>79</v>
       </c>
@@ -2261,7 +2238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>82</v>
       </c>
@@ -2270,7 +2247,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>84</v>
       </c>
@@ -2281,7 +2258,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>87</v>
       </c>
@@ -2292,7 +2269,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>90</v>
       </c>
@@ -2303,7 +2280,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>93</v>
       </c>
@@ -2314,7 +2291,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>96</v>
       </c>
@@ -2325,7 +2302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
@@ -2336,7 +2313,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
         <v>102</v>
       </c>
@@ -2347,7 +2324,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="8" t="s">
         <v>82</v>
       </c>
@@ -2356,7 +2333,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
         <v>106</v>
       </c>
@@ -2367,7 +2344,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="8" t="s">
         <v>109</v>
       </c>
@@ -2378,7 +2355,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="8" t="s">
         <v>112</v>
       </c>
@@ -2389,7 +2366,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="8" t="s">
         <v>115</v>
       </c>
@@ -2400,7 +2377,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="8" t="s">
         <v>118</v>
       </c>
@@ -2411,7 +2388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="8" t="s">
         <v>121</v>
       </c>
@@ -2422,7 +2399,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="8" t="s">
         <v>124</v>
       </c>
@@ -2433,7 +2410,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="8" t="s">
         <v>127</v>
       </c>
@@ -2444,7 +2421,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="8" t="s">
         <v>130</v>
       </c>
@@ -2455,7 +2432,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="8" t="s">
         <v>133</v>
       </c>
@@ -2466,7 +2443,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="8" t="s">
         <v>136</v>
       </c>
@@ -2477,7 +2454,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="8" t="s">
         <v>139</v>
       </c>
@@ -2488,7 +2465,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="8" t="s">
         <v>82</v>
       </c>
@@ -2497,7 +2474,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
         <v>143</v>
       </c>
@@ -2508,7 +2485,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
         <v>146</v>
       </c>
@@ -2519,7 +2496,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="8" t="s">
         <v>149</v>
       </c>
@@ -2530,7 +2507,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="8" t="s">
         <v>152</v>
       </c>
@@ -2541,7 +2518,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="8" t="s">
         <v>155</v>
       </c>
@@ -2552,7 +2529,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="8" t="s">
         <v>158</v>
       </c>
@@ -2563,7 +2540,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="8" t="s">
         <v>161</v>
       </c>
@@ -2574,7 +2551,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="8" t="s">
         <v>164</v>
       </c>
@@ -2585,7 +2562,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="8" t="s">
         <v>167</v>
       </c>
@@ -2596,7 +2573,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="8" t="s">
         <v>170</v>
       </c>
@@ -2607,7 +2584,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="8" t="s">
         <v>173</v>
       </c>
@@ -2618,7 +2595,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="8" t="s">
         <v>176</v>
       </c>
@@ -2629,7 +2606,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
         <v>179</v>
       </c>
@@ -2640,7 +2617,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="8" t="s">
         <v>182</v>
       </c>
@@ -2651,7 +2628,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
         <v>185</v>
       </c>
@@ -2662,7 +2639,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="8" t="s">
         <v>188</v>
       </c>
@@ -2673,7 +2650,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="8" t="s">
         <v>191</v>
       </c>
@@ -2684,7 +2661,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="8" t="s">
         <v>194</v>
       </c>
@@ -2695,7 +2672,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="8" t="s">
         <v>197</v>
       </c>
@@ -2706,7 +2683,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="8" t="s">
         <v>200</v>
       </c>
@@ -2717,7 +2694,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="8" t="s">
         <v>203</v>
       </c>
@@ -2728,7 +2705,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="8" t="s">
         <v>206</v>
       </c>
@@ -2739,7 +2716,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="8" t="s">
         <v>209</v>
       </c>
@@ -2750,7 +2727,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="8" t="s">
         <v>212</v>
       </c>
@@ -2761,7 +2738,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="8" t="s">
         <v>215</v>
       </c>
@@ -2772,7 +2749,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="8" t="s">
         <v>218</v>
       </c>
@@ -2783,7 +2760,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="8" t="s">
         <v>221</v>
       </c>
@@ -2794,7 +2771,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="8" t="s">
         <v>224</v>
       </c>
@@ -2805,7 +2782,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="8" t="s">
         <v>227</v>
       </c>
@@ -2816,7 +2793,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" s="8" t="s">
         <v>230</v>
       </c>
@@ -2827,7 +2804,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" s="8" t="s">
         <v>233</v>
       </c>
@@ -2838,7 +2815,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" s="8" t="s">
         <v>236</v>
       </c>
@@ -2849,7 +2826,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="8" t="s">
         <v>239</v>
       </c>
@@ -2860,7 +2837,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="8" t="s">
         <v>242</v>
       </c>
@@ -2871,7 +2848,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="8" t="s">
         <v>245</v>
       </c>
@@ -2882,7 +2859,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" s="8" t="s">
         <v>248</v>
       </c>
@@ -2893,7 +2870,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" s="8" t="s">
         <v>251</v>
       </c>
@@ -2904,7 +2881,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="8" t="s">
         <v>254</v>
       </c>
@@ -2915,7 +2892,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="8" t="s">
         <v>257</v>
       </c>
@@ -2926,7 +2903,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="8" t="s">
         <v>260</v>
       </c>
@@ -2937,7 +2914,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="8" t="s">
         <v>263</v>
       </c>
@@ -2948,7 +2925,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="8" t="s">
         <v>266</v>
       </c>
@@ -2959,7 +2936,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" s="8" t="s">
         <v>269</v>
       </c>
@@ -2970,7 +2947,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="8" t="s">
         <v>272</v>
       </c>
@@ -2981,7 +2958,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="8" t="s">
         <v>275</v>
       </c>
@@ -2992,7 +2969,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" s="8" t="s">
         <v>278</v>
       </c>
@@ -3003,7 +2980,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" s="8" t="s">
         <v>281</v>
       </c>
@@ -3014,7 +2991,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" s="8" t="s">
         <v>284</v>
       </c>
@@ -3025,7 +3002,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="8" t="s">
         <v>287</v>
       </c>
@@ -3036,7 +3013,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="8" t="s">
         <v>290</v>
       </c>
@@ -3047,7 +3024,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="8" t="s">
         <v>293</v>
       </c>
@@ -3058,7 +3035,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="8" t="s">
         <v>296</v>
       </c>
@@ -3069,7 +3046,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="8" t="s">
         <v>299</v>
       </c>
@@ -3080,7 +3057,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="8" t="s">
         <v>302</v>
       </c>
@@ -3091,7 +3068,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="8" t="s">
         <v>305</v>
       </c>
@@ -3102,7 +3079,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="8" t="s">
         <v>308</v>
       </c>
@@ -3113,7 +3090,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="8" t="s">
         <v>311</v>
       </c>
@@ -3135,74 +3112,489 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEEB26D-9786-4470-A8AD-43264E85ECB9}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="150.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="B2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="B4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="B5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="B8" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="B9" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="B10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>460</v>
+        <v>342</v>
+      </c>
+      <c r="B11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>350</v>
+      </c>
+      <c r="B16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>362</v>
+      </c>
+      <c r="B22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>364</v>
+      </c>
+      <c r="B23" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>366</v>
+      </c>
+      <c r="B24" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>370</v>
+      </c>
+      <c r="B26" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>372</v>
+      </c>
+      <c r="B27" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>372</v>
+      </c>
+      <c r="B28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F3B6E1-C926-490E-B179-CA4119029E15}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="134.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3214,510 +3606,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="150.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>318</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>321</v>
-      </c>
-      <c r="B4" t="s">
-        <v>322</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>327</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>330</v>
-      </c>
-      <c r="B7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>333</v>
-      </c>
-      <c r="B8" t="s">
-        <v>334</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>336</v>
-      </c>
-      <c r="B9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>339</v>
-      </c>
-      <c r="B10" t="s">
-        <v>340</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>342</v>
-      </c>
-      <c r="B11" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>344</v>
-      </c>
-      <c r="B12" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>346</v>
-      </c>
-      <c r="B13" t="s">
-        <v>347</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>348</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>350</v>
-      </c>
-      <c r="B16" t="s">
-        <v>351</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>354</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>356</v>
-      </c>
-      <c r="B19" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>358</v>
-      </c>
-      <c r="B20" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>360</v>
-      </c>
-      <c r="B21" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>362</v>
-      </c>
-      <c r="B22" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>364</v>
-      </c>
-      <c r="B23" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>366</v>
-      </c>
-      <c r="B24" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>368</v>
-      </c>
-      <c r="B25" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>370</v>
-      </c>
-      <c r="B26" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>372</v>
-      </c>
-      <c r="B27" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>372</v>
-      </c>
-      <c r="B28" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F3B6E1-C926-490E-B179-CA4119029E15}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="134.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
-        <v>314</v>
-      </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>411</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
@@ -3725,17 +3622,17 @@
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
         <v>412</v>
       </c>
@@ -3746,7 +3643,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>413</v>
       </c>
@@ -3757,7 +3654,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>414</v>
       </c>
@@ -3767,7 +3664,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>415</v>
       </c>
@@ -3777,7 +3674,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>416</v>
       </c>
@@ -3787,7 +3684,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>417</v>
       </c>
@@ -3797,7 +3694,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>418</v>
       </c>
@@ -3807,7 +3704,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>419</v>
       </c>
@@ -3817,7 +3714,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>420</v>
       </c>
@@ -3831,7 +3728,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>424</v>
       </c>
@@ -3845,7 +3742,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="C12" s="6" t="s">
         <v>428</v>
       </c>
@@ -3853,7 +3750,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="6" t="s">
         <v>430</v>
       </c>
@@ -3861,7 +3758,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="C14" s="6" t="s">
         <v>432</v>
       </c>
@@ -3869,7 +3766,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="C15" s="6" t="s">
         <v>434</v>
       </c>
@@ -3877,7 +3774,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="C16" s="6" t="s">
         <v>436</v>
       </c>
@@ -3885,7 +3782,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="C17" s="6" t="s">
         <v>438</v>
       </c>
@@ -3893,7 +3790,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="C18" s="6" t="s">
         <v>440</v>
       </c>
@@ -3901,7 +3798,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="C19" s="1" t="s">
         <v>442</v>
       </c>
@@ -3909,7 +3806,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4">
       <c r="C20" s="1" t="s">
         <v>444</v>
       </c>
@@ -3917,7 +3814,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4">
       <c r="C21" s="1" t="s">
         <v>446</v>
       </c>
@@ -3925,7 +3822,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4">
       <c r="C22" s="1" t="s">
         <v>448</v>
       </c>
@@ -3933,22 +3830,22 @@
         <v>449</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4">
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3">
       <c r="C33" s="1"/>
     </row>
   </sheetData>
@@ -3961,6 +3858,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
     <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
@@ -4189,60 +4106,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20F53162-DA3D-49C7-BB54-6E566081E5DD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f1000b3d-15af-42f4-8b30-1751694c7388"/>
-    <ds:schemaRef ds:uri="0a44024f-7437-4220-82e3-7a609f3cc5d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
 </file>
</xml_diff>

<commit_message>
možnost nastavit ip přímo, oprava databaze svetel, prace na kontext menu
</commit_message>
<xml_diff>
--- a/TRIMAZKON/Sharepoint_databaze.xlsx
+++ b/TRIMAZKON/Sharepoint_databaze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub.hlavacek.local\Desktop\JHV\Work\catalogue_manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0FDF745-B05A-43DC-A82C-1358DC1737DF}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{5854EDA4-EDB7-4482-88EE-7784F287C2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C2B115B-2DA3-42AC-90F4-25CE9736CD0F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontrolery" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Kamery" sheetId="3" r:id="rId3"/>
     <sheet name="Kabely" sheetId="7" r:id="rId4"/>
     <sheet name="Přislušenství" sheetId="4" r:id="rId5"/>
+    <sheet name="Světla" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="461">
   <si>
     <t>Omron FZ/FH</t>
   </si>
@@ -1403,6 +1404,39 @@
   </si>
   <si>
     <t>EtherNet/IP module</t>
+  </si>
+  <si>
+    <t>CL-50</t>
+  </si>
+  <si>
+    <t>světlo</t>
+  </si>
+  <si>
+    <t>BL-50W-4S</t>
+  </si>
+  <si>
+    <t>LA-70B</t>
+  </si>
+  <si>
+    <t>LA-70W</t>
+  </si>
+  <si>
+    <t>LA-120W</t>
+  </si>
+  <si>
+    <t>DL-120W-HI</t>
+  </si>
+  <si>
+    <t>LL-130W</t>
+  </si>
+  <si>
+    <t>DLU-140W-HI</t>
+  </si>
+  <si>
+    <t>FL-MD90MC</t>
+  </si>
+  <si>
+    <t>SP-27IR-850</t>
   </si>
 </sst>
 </file>
@@ -3610,14 +3644,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="46.140625" customWidth="1"/>
   </cols>
@@ -3857,27 +3891,92 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B43BF8-D338-4CD8-9175-B60668AB06F9}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100AC30A1654071464B83845798603538A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="9168d1d45adf597786ba4404c21a0f63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f1000b3d-15af-42f4-8b30-1751694c7388" xmlns:ns3="0a44024f-7437-4220-82e3-7a609f3cc5d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2a603704bc0fe2974ac9a36df3b95205" ns2:_="" ns3:_="">
     <xsd:import namespace="f1000b3d-15af-42f4-8b30-1751694c7388"/>
@@ -4106,8 +4205,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f1000b3d-15af-42f4-8b30-1751694c7388" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0a44024f-7437-4220-82e3-7a609f3cc5d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4115,5 +4234,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4401364-4573-4AA3-A01C-3A51337634B0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB475825-C6B0-46AE-A469-0210B2AABFAD}"/>
 </file>
</xml_diff>